<commit_message>
removed the results on recycling from the pptx and xlsx files
</commit_message>
<xml_diff>
--- a/baseline/2slides_for_Berber/Results_summary_Table.xlsx
+++ b/baseline/2slides_for_Berber/Results_summary_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/L.Nabwire/git/Maize_Uganda/mippi_UG/baseline/2slides_for_Berber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72FFD493-1621-430E-A07B-503979D03252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{72FFD493-1621-430E-A07B-503979D03252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98998C3C-7095-4C7B-A953-3DA793CD2A41}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -288,10 +288,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,9 +469,16 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'1st slide'!$A$3:$B$11</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'1st slide'!$A$3:$B$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'1st slide'!$A$3:$B$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>All improved varieties</c:v>
@@ -491,15 +498,6 @@
                   <c:pt idx="5">
                     <c:v>OPVs only</c:v>
                   </c:pt>
-                  <c:pt idx="6">
-                    <c:v>All improved varieties</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Hybrids only</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>OPVs only</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -508,19 +506,23 @@
                   <c:pt idx="3">
                     <c:v>Number of years the farmer has used the variety</c:v>
                   </c:pt>
-                  <c:pt idx="6">
-                    <c:v>% of farmers who recycle seed more than the recommended (0 times for hydrids &amp; 3 times for OPVs)</c:v>
-                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1st slide'!$C$3:$C$11</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'1st slide'!$C$3:$C$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'1st slide'!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40.299999999999997</c:v>
                 </c:pt>
@@ -538,15 +540,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>13.62</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>91.66</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>99.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>77.06</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -640,9 +633,16 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'1st slide'!$A$3:$B$11</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'1st slide'!$A$3:$B$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'1st slide'!$A$3:$B$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>All improved varieties</c:v>
@@ -662,15 +662,6 @@
                   <c:pt idx="5">
                     <c:v>OPVs only</c:v>
                   </c:pt>
-                  <c:pt idx="6">
-                    <c:v>All improved varieties</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Hybrids only</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>OPVs only</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -679,19 +670,23 @@
                   <c:pt idx="3">
                     <c:v>Number of years the farmer has used the variety</c:v>
                   </c:pt>
-                  <c:pt idx="6">
-                    <c:v>% of farmers who recycle seed more than the recommended (0 times for hydrids &amp; 3 times for OPVs)</c:v>
-                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1st slide'!$D$3:$D$11</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'1st slide'!$D$3:$D$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'1st slide'!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>26.11</c:v>
                 </c:pt>
@@ -709,15 +704,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.09</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>86.81</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>98.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>66.040000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,9 +797,16 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'1st slide'!$A$3:$B$11</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'1st slide'!$A$3:$B$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'1st slide'!$A$3:$B$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>All improved varieties</c:v>
@@ -833,15 +826,6 @@
                   <c:pt idx="5">
                     <c:v>OPVs only</c:v>
                   </c:pt>
-                  <c:pt idx="6">
-                    <c:v>All improved varieties</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Hybrids only</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>OPVs only</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -850,19 +834,23 @@
                   <c:pt idx="3">
                     <c:v>Number of years the farmer has used the variety</c:v>
                   </c:pt>
-                  <c:pt idx="6">
-                    <c:v>% of farmers who recycle seed more than the recommended (0 times for hydrids &amp; 3 times for OPVs)</c:v>
-                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1st slide'!$E$3:$E$11</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'1st slide'!$E$3:$E$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'1st slide'!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>43.96</c:v>
                 </c:pt>
@@ -880,15 +868,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>15.38</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>92.47</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>99.13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>79.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -967,7 +946,7 @@
         <c:axId val="573606256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
+          <c:max val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1031,6 +1010,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.3099055007130445E-2"/>
+          <c:y val="0.93636962973508697"/>
+          <c:w val="0.85380166802616908"/>
+          <c:h val="3.8595599750309378E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1044,7 +1033,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1688,10 +1677,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1958,7 +1943,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1975,12 +1960,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="C2" s="5" t="s">
@@ -2006,7 +1991,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -2036,7 +2021,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -2064,7 +2049,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="18"/>
+      <c r="A5" s="17"/>
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -2092,7 +2077,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
@@ -2122,7 +2107,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="18"/>
+      <c r="A7" s="17"/>
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -2150,7 +2135,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="18"/>
+      <c r="A8" s="17"/>
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -2178,7 +2163,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B9" t="s">
@@ -2208,7 +2193,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="18"/>
+      <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -2236,7 +2221,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="18"/>
+      <c r="A11" s="17"/>
       <c r="B11" t="s">
         <v>24</v>
       </c>

</xml_diff>